<commit_message>
Update Export standard: fix bug + migrate from POI to Xlxs4J
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_v1.1.xlsx
+++ b/src/main/webapp/WEB-INF/data/TL_TRICKService_NormImport_v1.1.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eomar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eomar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="28620" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14417" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NormInfo" sheetId="1" r:id="rId1"/>
     <sheet name="NormData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -41,30 +40,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>1.1.1</t>
-  </si>
-  <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
-    <t>gtkgol</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>nkdezoniz</t>
-  </si>
-  <si>
-    <t>cù</t>
-  </si>
-  <si>
     <t>Standard for test</t>
   </si>
   <si>
@@ -81,34 +56,13 @@
   </si>
   <si>
     <t>Description_FRA</t>
-  </si>
-  <si>
-    <t>Level 1 domain</t>
-  </si>
-  <si>
-    <t>Level 1 description</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Level 2 domain</t>
-  </si>
-  <si>
-    <t>Level 2 description</t>
-  </si>
-  <si>
-    <t>Level 3 domain</t>
-  </si>
-  <si>
-    <t>Level 3 description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,16 +70,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,20 +101,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -168,7 +208,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TableNormInfo" displayName="TableNormInfo" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="1"/>
+    <tableColumn id="1" name="Name" dataDxfId="4"/>
     <tableColumn id="2" name="Version"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="Computable"/>
@@ -178,11 +218,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G6" totalsRowShown="0">
-  <autoFilter ref="A1:G6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TableNormData" displayName="TableNormData" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:G2"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Level"/>
-    <tableColumn id="2" name="Reference" dataDxfId="0"/>
+    <tableColumn id="2" name="Reference" dataDxfId="1"/>
     <tableColumn id="3" name="Computable"/>
     <tableColumn id="4" name="Domain_ENG"/>
     <tableColumn id="5" name="Description_ENG"/>
@@ -520,15 +560,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.3828125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.3046875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,15 +582,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>2015</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -566,137 +606,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.3046875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.84375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.15234375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.3828125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>